<commit_message>
Finish up excel import
</commit_message>
<xml_diff>
--- a/odoo/custom/src/private/nxpo_budget_control_excel/templates/budget_control.xlsx
+++ b/odoo/custom/src/private/nxpo_budget_control_excel/templates/budget_control.xlsx
@@ -10,6 +10,7 @@
   <sheets>
     <sheet name="BudgetControl" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="RawData" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="AG" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -190,7 +191,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -265,6 +266,18 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -355,7 +368,7 @@
   <dimension ref="A1:AMJ1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1941,18 +1954,19 @@
       <c r="N100" s="18"/>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="16"/>
-      <c r="C101" s="16"/>
-      <c r="D101" s="17"/>
-      <c r="E101" s="16"/>
-      <c r="F101" s="16"/>
-      <c r="G101" s="16"/>
-      <c r="H101" s="16"/>
-      <c r="I101" s="16"/>
-      <c r="J101" s="16"/>
-      <c r="K101" s="16"/>
-      <c r="L101" s="16"/>
-      <c r="M101" s="17"/>
+      <c r="A101" s="19"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="20"/>
+      <c r="D101" s="21"/>
+      <c r="E101" s="20"/>
+      <c r="F101" s="20"/>
+      <c r="G101" s="20"/>
+      <c r="H101" s="20"/>
+      <c r="I101" s="20"/>
+      <c r="J101" s="20"/>
+      <c r="K101" s="20"/>
+      <c r="L101" s="20"/>
+      <c r="M101" s="21"/>
       <c r="N101" s="18"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15450,6 +15464,12 @@
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="M5:N5"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A9:A100" type="list">
+      <formula1>AG!$A:$A</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -15471,127 +15491,127 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="19"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="23"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="23"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="20"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="23"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="20"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="23"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="20"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="23"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="23"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="23"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="23"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="20"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="20"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="23"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="23"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="23"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="23"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="23"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="23"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="23"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="23"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="23"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="23"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
+      <c r="A24" s="22"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="23"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -15602,4 +15622,27 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>